<commit_message>
make vert and edge write to file as well as print to cout
</commit_message>
<xml_diff>
--- a/GraphProfile Analysis/Parallelization Analysis/Runtime Data.xlsx
+++ b/GraphProfile Analysis/Parallelization Analysis/Runtime Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="11052" windowHeight="9132" activeTab="2"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="11052" windowHeight="9132" tabRatio="808" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="raw data" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="% improvement, &lt;1s removed" sheetId="3" r:id="rId3"/>
     <sheet name="% improvement, &lt;1s kept" sheetId="5" r:id="rId4"/>
     <sheet name="abc, by vertex chosen" sheetId="4" r:id="rId5"/>
+    <sheet name="bc anomaly" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="45">
   <si>
     <t>On linux.student.cs.uwaterloo.ca machines</t>
   </si>
@@ -104,6 +105,9 @@
     <t>command</t>
   </si>
   <si>
+    <t>raw</t>
+  </si>
+  <si>
     <t>graph:</t>
   </si>
   <si>
@@ -135,6 +139,21 @@
   </si>
   <si>
     <t>% improvement</t>
+  </si>
+  <si>
+    <t>average of averages(by graph)</t>
+  </si>
+  <si>
+    <t>average of averages(by command0</t>
+  </si>
+  <si>
+    <t>average of all datapoints</t>
+  </si>
+  <si>
+    <t>vertices</t>
+  </si>
+  <si>
+    <t>loops</t>
   </si>
 </sst>
 </file>
@@ -7091,12 +7110,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="M88" sqref="M88:M89"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
     <col min="3" max="4" width="13.21875" customWidth="1"/>
   </cols>
@@ -7119,7 +7139,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -8393,7 +8413,7 @@
         <v>9.1573033707865168</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H81">
         <v>175</v>
       </c>
@@ -8415,12 +8435,12 @@
         <v>7.6210526315789471</v>
       </c>
     </row>
-    <row r="82" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>4</v>
       </c>
@@ -8440,8 +8460,11 @@
         <f>AVERAGE(M6:M87)</f>
         <v>16.97083906297145</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O88" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -8461,78 +8484,174 @@
         <f>_xlfn.STDEV.S(M6:M87)</f>
         <v>11.230235550378003</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O89">
+        <f>AVERAGE(D88:M88)</f>
+        <v>19.570698354891388</v>
+      </c>
+      <c r="P89">
+        <f>_xlfn.STDEV.S(D88:M88)</f>
+        <v>2.6276213964411244</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O90" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O91">
+        <f>AVERAGE(O77,O72,O6:O67)</f>
+        <v>18.901849130734583</v>
+      </c>
+      <c r="P91">
+        <f>_xlfn.STDEV.S(O6:O80)</f>
+        <v>8.9422157408131362</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="B92">
+        <v>6.2386395895770885</v>
+      </c>
+      <c r="C92">
+        <v>0.28019675609793682</v>
+      </c>
+      <c r="O92" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="B93">
+        <v>9.1774685678436523</v>
+      </c>
+      <c r="C93">
+        <v>3.0216709363038112</v>
+      </c>
+      <c r="O93">
+        <f>AVERAGE(M67:M81,J67:J81,M44:M56,D34:D38,G34,M24:M28,J24:J28,G24:G28,M6:M23,J6:J14,G6:G14,G67:G71)</f>
+        <v>18.825781070594498</v>
+      </c>
+      <c r="P93">
+        <f>_xlfn.STDEV.S((M67:M81,J67:J81,M44:M56,D34:D38,G34,M24:M28,J24:J28,G24:G28,M6:M23,J6:J14,G6:G14,G67:G71))</f>
+        <v>11.220290969593869</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="B94">
+        <v>16.185405161360421</v>
+      </c>
+      <c r="C94">
+        <v>10.745564773172298</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="B95">
+        <v>19.666666666666668</v>
+      </c>
+      <c r="C95">
+        <v>4.4534630719624477</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="B96">
+        <v>19.706349206349202</v>
+      </c>
+      <c r="C96">
+        <v>6.4492905385392101</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="B97">
+        <v>21.575779727095519</v>
+      </c>
+      <c r="C97">
+        <v>6.191650399892322</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="B98">
+        <v>23.354166666666668</v>
+      </c>
+      <c r="C98">
+        <v>9.9572249831506454</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="B99">
+        <v>35.310317460317464</v>
+      </c>
+      <c r="C99">
+        <v>5.0325038146241425</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>2</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>4039</v>
+      </c>
+      <c r="B102">
+        <v>23.23</v>
+      </c>
+      <c r="C102">
+        <v>8.5176366735687825</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>36692</v>
+      </c>
+      <c r="B103">
+        <v>19.007685350746147</v>
+      </c>
+      <c r="C103">
+        <v>13.147599015966225</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>75888</v>
+      </c>
+      <c r="B104">
+        <v>16.97083906297145</v>
+      </c>
+      <c r="C104">
+        <v>11.230235550378003</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A92:C99">
+    <sortCondition ref="B92:B99"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8541,8 +8660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8569,7 +8688,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -9848,10 +9967,10 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -9863,15 +9982,15 @@
       <c r="J1" s="3"/>
       <c r="K1" s="4"/>
       <c r="O1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="6">
         <v>11</v>
@@ -9894,27 +10013,27 @@
       </c>
       <c r="K2" s="7"/>
       <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" t="s">
-        <v>30</v>
-      </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
@@ -9962,10 +10081,10 @@
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -10165,10 +10284,10 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -10180,15 +10299,15 @@
       <c r="J9" s="3"/>
       <c r="K9" s="4"/>
       <c r="O9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="6">
         <v>11</v>
@@ -10211,27 +10330,27 @@
       </c>
       <c r="K10" s="7"/>
       <c r="O10" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" t="s">
         <v>31</v>
       </c>
-      <c r="P10" t="s">
-        <v>30</v>
-      </c>
       <c r="Q10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="6">
         <v>1</v>
@@ -10279,10 +10398,10 @@
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -10482,10 +10601,10 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -10499,15 +10618,15 @@
       <c r="L17" s="3"/>
       <c r="M17" s="4"/>
       <c r="O17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6">
         <v>11</v>
@@ -10534,27 +10653,27 @@
       </c>
       <c r="M18" s="7"/>
       <c r="O18" t="s">
+        <v>32</v>
+      </c>
+      <c r="P18" t="s">
         <v>31</v>
       </c>
-      <c r="P18" t="s">
-        <v>30</v>
-      </c>
       <c r="Q18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
@@ -10606,10 +10725,10 @@
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -10864,4 +10983,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="14.77734375" style="6" customWidth="1"/>
+    <col min="3" max="4" width="13.21875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="6">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6">
+        <f>AVERAGE(B4:B10)</f>
+        <v>342.14285714285717</v>
+      </c>
+      <c r="C2" s="6">
+        <f t="shared" ref="C2:D2" si="0">AVERAGE(C4:C10)</f>
+        <v>18</v>
+      </c>
+      <c r="D2" s="6">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6">
+        <f>_xlfn.STDEV.S(B4:B10)</f>
+        <v>15.710172621888146</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:D3" si="1">_xlfn.STDEV.S(C4:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="shared" si="1"/>
+        <v>4.5460605656619517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6">
+        <v>327</v>
+      </c>
+      <c r="C4" s="6">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="6">
+        <v>371</v>
+      </c>
+      <c r="C5" s="6">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="11">
+        <v>350</v>
+      </c>
+      <c r="C6" s="11">
+        <v>18</v>
+      </c>
+      <c r="D6" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="11">
+        <v>339</v>
+      </c>
+      <c r="D7" s="11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="11">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="11">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="11">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>